<commit_message>
correcciones codigo y aprox3 terminada
</commit_message>
<xml_diff>
--- a/entrenamiento/resultados/Aproximacion3.xlsx
+++ b/entrenamiento/resultados/Aproximacion3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,6 +596,40 @@
         <v>0.0513337030217291</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.03023541361821315</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.01458826870677125</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.2060187776853033</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.05781738456804626</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.01876863687217622</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01047510069578992</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1632211676552942</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.05209583186486728</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>